<commit_message>
Fase de riesgos y costos
actualizacion de documentos
</commit_message>
<xml_diff>
--- a/Administracion-de-Proyectos/Planeacion-del-proyecto/TMv3-BD de Riesgos.xlsx
+++ b/Administracion-de-Proyectos/Planeacion-del-proyecto/TMv3-BD de Riesgos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="404">
   <si>
     <t>Versión</t>
   </si>
@@ -1159,6 +1159,75 @@
   </si>
   <si>
     <t>El tester  que prueba el  módulo es el  mismo que lo realizo</t>
+  </si>
+  <si>
+    <t>MMC_031</t>
+  </si>
+  <si>
+    <t>MMC_032</t>
+  </si>
+  <si>
+    <t>MMC_033</t>
+  </si>
+  <si>
+    <t>MMC_034</t>
+  </si>
+  <si>
+    <t>MMC_035</t>
+  </si>
+  <si>
+    <t>MMC_036</t>
+  </si>
+  <si>
+    <t>MMC_037</t>
+  </si>
+  <si>
+    <t>MMC_038</t>
+  </si>
+  <si>
+    <t>MMC_039</t>
+  </si>
+  <si>
+    <t>MMC_040</t>
+  </si>
+  <si>
+    <t>MMC_041</t>
+  </si>
+  <si>
+    <t>MMC_042</t>
+  </si>
+  <si>
+    <t>MMC_043</t>
+  </si>
+  <si>
+    <t>MMC_044</t>
+  </si>
+  <si>
+    <t>MMC_045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adquirir una plantilla base para el proceso </t>
+  </si>
+  <si>
+    <t>Definir y dar a conocer las políticas del proyecto a todos los participantes</t>
+  </si>
+  <si>
+    <t>Establecer un proceso de control</t>
+  </si>
+  <si>
+    <t>Elección de otro proveedor de servicios</t>
+  </si>
+  <si>
+    <t>Realizar pruebas exhaustivas al producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilizar herramientas software previamente conocido </t>
+  </si>
+  <si>
+    <t>Verificar y validar la documentación</t>
+  </si>
+  <si>
+    <t>Buscar software alternativo que cubra la necesidad que sea de uso libre</t>
   </si>
 </sst>
 </file>
@@ -1425,7 +1494,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1561,6 +1630,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1585,16 +1660,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2076,40 +2148,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="53" t="s">
         <v>350</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="54"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="52"/>
-      <c r="B2" s="52"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="54"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="52"/>
-      <c r="B3" s="52"/>
+      <c r="A3" s="54"/>
+      <c r="B3" s="54"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="52"/>
-      <c r="B4" s="52"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="52"/>
-      <c r="B5" s="52"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="52"/>
-      <c r="B6" s="52"/>
+      <c r="A6" s="54"/>
+      <c r="B6" s="54"/>
     </row>
     <row r="7" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="53"/>
+      <c r="B7" s="55"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="53"/>
-      <c r="B8" s="53"/>
+      <c r="A8" s="55"/>
+      <c r="B8" s="55"/>
     </row>
     <row r="9" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
@@ -2165,10 +2237,10 @@
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="54" t="s">
+      <c r="A17" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="55"/>
+      <c r="B17" s="57"/>
     </row>
     <row r="18" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
@@ -2194,10 +2266,10 @@
       <c r="A21" s="30"/>
     </row>
     <row r="22" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="54" t="s">
+      <c r="A22" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="55"/>
+      <c r="B22" s="57"/>
     </row>
     <row r="23" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
@@ -2223,12 +2295,12 @@
       <c r="A26" s="30"/>
     </row>
     <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="54" t="s">
+      <c r="A27" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="56"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="55"/>
+      <c r="B27" s="58"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="57"/>
     </row>
     <row r="28" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
@@ -2313,8 +2385,8 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="12"/>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
       <c r="F1" s="12"/>
@@ -2322,8 +2394,8 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
@@ -2331,8 +2403,8 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="12"/>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
@@ -2340,8 +2412,8 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -2349,8 +2421,8 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
@@ -2358,19 +2430,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="58"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="60"/>
       <c r="D7" s="13"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
@@ -4058,8 +4130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4091,11 +4163,11 @@
       <c r="G2"/>
     </row>
     <row r="3" spans="1:7" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="60"/>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
       <c r="F3"/>
       <c r="G3"/>
     </row>
@@ -4127,11 +4199,11 @@
       <c r="G6"/>
     </row>
     <row r="7" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="62" t="s">
         <v>202</v>
       </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
       <c r="D7" s="1"/>
       <c r="E7"/>
       <c r="F7"/>
@@ -4147,13 +4219,13 @@
       <c r="G8"/>
     </row>
     <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="51" t="s">
         <v>17</v>
       </c>
       <c r="D9"/>
@@ -4498,69 +4570,171 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="8"/>
-      <c r="C40" s="7"/>
+      <c r="A40" s="52" t="s">
+        <v>381</v>
+      </c>
+      <c r="B40" s="52" t="s">
+        <v>264</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="C41"/>
+      <c r="A41" s="52" t="s">
+        <v>382</v>
+      </c>
+      <c r="B41" s="52" t="s">
+        <v>264</v>
+      </c>
+      <c r="C41" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C42" s="7"/>
+      <c r="A42" s="52" t="s">
+        <v>383</v>
+      </c>
+      <c r="B42" s="52" t="s">
+        <v>265</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C43" s="7"/>
+      <c r="A43" s="52" t="s">
+        <v>384</v>
+      </c>
+      <c r="B43" s="52" t="s">
+        <v>265</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>398</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="7"/>
+      <c r="A44" s="52" t="s">
+        <v>385</v>
+      </c>
+      <c r="B44" s="52" t="s">
+        <v>264</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>399</v>
+      </c>
     </row>
     <row r="45" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
+      <c r="A45" s="52" t="s">
+        <v>386</v>
+      </c>
+      <c r="B45" s="52" t="s">
+        <v>265</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>401</v>
+      </c>
     </row>
     <row r="46" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="8"/>
-      <c r="B46" s="8"/>
+      <c r="A46" s="52" t="s">
+        <v>387</v>
+      </c>
+      <c r="B46" s="52" t="s">
+        <v>264</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="8"/>
-      <c r="B47" s="8"/>
+      <c r="A47" s="52" t="s">
+        <v>388</v>
+      </c>
+      <c r="B47" s="52" t="s">
+        <v>265</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="8"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="8"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="8"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="52" t="s">
+        <v>389</v>
+      </c>
+      <c r="B48" s="52" t="s">
+        <v>264</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="52" t="s">
+        <v>390</v>
+      </c>
+      <c r="B49" s="52" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="52" t="s">
+        <v>391</v>
+      </c>
+      <c r="B50" s="52" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="52" t="s">
+        <v>392</v>
+      </c>
+      <c r="B51" s="52" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="52" t="s">
+        <v>393</v>
+      </c>
+      <c r="B52" s="52" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="52" t="s">
+        <v>394</v>
+      </c>
+      <c r="B53" s="52" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="52" t="s">
+        <v>395</v>
+      </c>
+      <c r="B54" s="52" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="8"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="8"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="8"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="8"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="8"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="8"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="8"/>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
@@ -4654,7 +4828,7 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:B39">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:B54">
       <formula1>"Mitigación, Contingencia"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>